<commit_message>
Improve bike yearly report
</commit_message>
<xml_diff>
--- a/comptages/report/template_yearly_arx.xlsx
+++ b/comptages/report/template_yearly_arx.xlsx
@@ -3729,8 +3729,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="14548112"/>
-        <c:axId val="98925265"/>
+        <c:axId val="6181507"/>
+        <c:axId val="88101351"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3880,11 +3880,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="14548112"/>
-        <c:axId val="98925265"/>
+        <c:axId val="6181507"/>
+        <c:axId val="88101351"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14548112"/>
+        <c:axId val="6181507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3950,7 +3950,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98925265"/>
+        <c:crossAx val="88101351"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3958,7 +3958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98925265"/>
+        <c:axId val="88101351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4034,7 +4034,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14548112"/>
+        <c:crossAx val="6181507"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4163,8 +4163,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="87212644"/>
-        <c:axId val="70129726"/>
+        <c:axId val="54607436"/>
+        <c:axId val="70624096"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4314,11 +4314,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="87212644"/>
-        <c:axId val="70129726"/>
+        <c:axId val="54607436"/>
+        <c:axId val="70624096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87212644"/>
+        <c:axId val="54607436"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4384,7 +4384,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70129726"/>
+        <c:crossAx val="70624096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4392,7 +4392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70129726"/>
+        <c:axId val="70624096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4468,7 +4468,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87212644"/>
+        <c:crossAx val="54607436"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4597,8 +4597,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="13124015"/>
-        <c:axId val="42760490"/>
+        <c:axId val="78552746"/>
+        <c:axId val="5733386"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4748,11 +4748,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="13124015"/>
-        <c:axId val="42760490"/>
+        <c:axId val="78552746"/>
+        <c:axId val="5733386"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13124015"/>
+        <c:axId val="78552746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4818,7 +4818,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42760490"/>
+        <c:crossAx val="5733386"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4826,7 +4826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42760490"/>
+        <c:axId val="5733386"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4902,7 +4902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13124015"/>
+        <c:crossAx val="78552746"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5031,8 +5031,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="15305027"/>
-        <c:axId val="37026326"/>
+        <c:axId val="66523577"/>
+        <c:axId val="2340145"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5182,11 +5182,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="15305027"/>
-        <c:axId val="37026326"/>
+        <c:axId val="66523577"/>
+        <c:axId val="2340145"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15305027"/>
+        <c:axId val="66523577"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5252,7 +5252,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37026326"/>
+        <c:crossAx val="2340145"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5260,7 +5260,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37026326"/>
+        <c:axId val="2340145"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5336,7 +5336,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15305027"/>
+        <c:crossAx val="66523577"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5465,8 +5465,8 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="0"/>
-        <c:axId val="78232746"/>
-        <c:axId val="46458878"/>
+        <c:axId val="30513170"/>
+        <c:axId val="64500352"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5616,11 +5616,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="78232746"/>
-        <c:axId val="46458878"/>
+        <c:axId val="30513170"/>
+        <c:axId val="64500352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78232746"/>
+        <c:axId val="30513170"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5686,7 +5686,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46458878"/>
+        <c:crossAx val="64500352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5694,7 +5694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46458878"/>
+        <c:axId val="64500352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5770,7 +5770,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78232746"/>
+        <c:crossAx val="30513170"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6269,11 +6269,11 @@
         </c:ser>
         <c:gapWidth val="2"/>
         <c:overlap val="100"/>
-        <c:axId val="88490483"/>
-        <c:axId val="69792714"/>
+        <c:axId val="95011166"/>
+        <c:axId val="64323416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88490483"/>
+        <c:axId val="95011166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6305,7 +6305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69792714"/>
+        <c:crossAx val="64323416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6313,7 +6313,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69792714"/>
+        <c:axId val="64323416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6389,7 +6389,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88490483"/>
+        <c:crossAx val="95011166"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6864,11 +6864,11 @@
         </c:ser>
         <c:gapWidth val="2"/>
         <c:overlap val="100"/>
-        <c:axId val="64882468"/>
-        <c:axId val="71424474"/>
+        <c:axId val="68988769"/>
+        <c:axId val="52774839"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64882468"/>
+        <c:axId val="68988769"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6900,7 +6900,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71424474"/>
+        <c:crossAx val="52774839"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6908,7 +6908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71424474"/>
+        <c:axId val="52774839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6984,7 +6984,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64882468"/>
+        <c:crossAx val="68988769"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7645,11 +7645,11 @@
         </c:ser>
         <c:gapWidth val="2"/>
         <c:overlap val="100"/>
-        <c:axId val="70013023"/>
-        <c:axId val="10324040"/>
+        <c:axId val="50705804"/>
+        <c:axId val="38198854"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70013023"/>
+        <c:axId val="50705804"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7681,7 +7681,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10324040"/>
+        <c:crossAx val="38198854"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7689,7 +7689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10324040"/>
+        <c:axId val="38198854"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7765,7 +7765,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70013023"/>
+        <c:crossAx val="50705804"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8426,11 +8426,11 @@
         </c:ser>
         <c:gapWidth val="2"/>
         <c:overlap val="100"/>
-        <c:axId val="74147027"/>
-        <c:axId val="9191932"/>
+        <c:axId val="70890856"/>
+        <c:axId val="20944762"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74147027"/>
+        <c:axId val="70890856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8462,7 +8462,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9191932"/>
+        <c:crossAx val="20944762"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8470,7 +8470,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9191932"/>
+        <c:axId val="20944762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8546,7 +8546,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74147027"/>
+        <c:crossAx val="70890856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8585,9 +8585,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>2520</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8596,7 +8596,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2676240"/>
-        <a:ext cx="6904800" cy="2912400"/>
+        <a:ext cx="6904440" cy="2912040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8620,9 +8620,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>612000</xdr:colOff>
+      <xdr:colOff>611640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8631,7 +8631,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2676240"/>
-        <a:ext cx="6899760" cy="2921760"/>
+        <a:ext cx="6899400" cy="2921400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8655,9 +8655,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>612000</xdr:colOff>
+      <xdr:colOff>611640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8666,7 +8666,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2676240"/>
-        <a:ext cx="6899760" cy="2921760"/>
+        <a:ext cx="6899400" cy="2921400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8690,9 +8690,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>612000</xdr:colOff>
+      <xdr:colOff>611640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8701,7 +8701,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2676240"/>
-        <a:ext cx="6899760" cy="2921760"/>
+        <a:ext cx="6899400" cy="2921400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8725,9 +8725,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>612000</xdr:colOff>
+      <xdr:colOff>611640</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8736,7 +8736,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2676240"/>
-        <a:ext cx="6899760" cy="2921760"/>
+        <a:ext cx="6899400" cy="2921400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8760,9 +8760,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>964440</xdr:colOff>
+      <xdr:colOff>964080</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8771,7 +8771,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2050920"/>
-        <a:ext cx="7522560" cy="4443120"/>
+        <a:ext cx="7518240" cy="4442760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8790,9 +8790,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>964440</xdr:colOff>
+      <xdr:colOff>964080</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8801,7 +8801,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="7820640"/>
-        <a:ext cx="7522560" cy="4443480"/>
+        <a:ext cx="7518240" cy="4443120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8825,9 +8825,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>673200</xdr:colOff>
+      <xdr:colOff>672840</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8836,7 +8836,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="2024280"/>
-        <a:ext cx="7559640" cy="4443840"/>
+        <a:ext cx="7565040" cy="4443480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8855,9 +8855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>673200</xdr:colOff>
+      <xdr:colOff>672840</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8866,7 +8866,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="7794360"/>
-        <a:ext cx="7559640" cy="4443840"/>
+        <a:ext cx="7565040" cy="4443480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8890,10 +8890,10 @@
       <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="119.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="119.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9000,7 +9000,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="8.71"/>
@@ -9725,7 +9725,7 @@
       <selection pane="topLeft" activeCell="R26" activeCellId="0" sqref="R26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="8.71"/>
@@ -10037,7 +10037,7 @@
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="7.29"/>
@@ -13256,10 +13256,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="1.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="178" width="11.42"/>
@@ -15899,13 +15899,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="1.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16886,13 +16886,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="1.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="178" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="178" width="9.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20250,13 +20250,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="2.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21338,7 +21338,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="7"/>
@@ -24779,7 +24779,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="2" style="1" width="7"/>
@@ -29450,9 +29450,9 @@
       <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.57"/>
@@ -32794,7 +32794,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -32945,7 +32945,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="1" style="1" width="11.57"/>
   </cols>
@@ -34470,7 +34470,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="1" style="1" width="11.57"/>
   </cols>
@@ -37785,7 +37785,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="8.71"/>
@@ -39077,10 +39077,10 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
+      <selection pane="topLeft" activeCell="M27" activeCellId="0" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="8.71"/>
@@ -39498,7 +39498,7 @@
       <selection pane="topLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="8.71"/>
@@ -40361,7 +40361,7 @@
       <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.31640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="8.71"/>

</xml_diff>